<commit_message>
Add membership for chemicals, groups, water, etc.
</commit_message>
<xml_diff>
--- a/fedelemflowlist/input/SecondaryContextMembership.xlsx
+++ b/fedelemflowlist/input/SecondaryContextMembership.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wingwers\Federal-LCA-Commons-Elementary-Flow-List\fedelemflowlist\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wesle\Dropbox\TD 4 Technical Work\Flow Context Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A39015-6AF5-4DFE-916A-A492B67E7B2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501A4456-E33C-444B-8955-AC90598B63E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" xr2:uid="{FBB5837A-FF81-4680-A9D9-CC7A0A70A54C}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{FBB5837A-FF81-4680-A9D9-CC7A0A70A54C}"/>
   </bookViews>
   <sheets>
     <sheet name="SecondaryContextMembership" sheetId="2" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="25">
   <si>
     <t>Vertical Strata</t>
   </si>
@@ -94,12 +95,24 @@
   <si>
     <t>ContextPreferred</t>
   </si>
+  <si>
+    <t>Geological</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Groups</t>
+  </si>
+  <si>
+    <t>Chemicals</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +124,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -136,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -148,6 +167,8 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,10 +483,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29F846F-F783-49D5-99B1-894124203F3B}">
-  <dimension ref="A1:AJ16"/>
+  <dimension ref="A1:AJ100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +502,7 @@
     <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.42578125" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
@@ -1307,7 +1329,3200 @@
         <v>1</v>
       </c>
     </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0</v>
+      </c>
+      <c r="K18" s="4">
+        <v>0</v>
+      </c>
+      <c r="L18" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0</v>
+      </c>
+      <c r="I19" s="4">
+        <v>0</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0</v>
+      </c>
+      <c r="K19" s="4">
+        <v>0</v>
+      </c>
+      <c r="L19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0</v>
+      </c>
+      <c r="K20" s="4">
+        <v>0</v>
+      </c>
+      <c r="L20" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0</v>
+      </c>
+      <c r="K21" s="4">
+        <v>0</v>
+      </c>
+      <c r="L21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0</v>
+      </c>
+      <c r="I22" s="4">
+        <v>0</v>
+      </c>
+      <c r="J22" s="4">
+        <v>0</v>
+      </c>
+      <c r="K22" s="4">
+        <v>0</v>
+      </c>
+      <c r="L22" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0</v>
+      </c>
+      <c r="I23" s="4">
+        <v>0</v>
+      </c>
+      <c r="J23" s="4">
+        <v>0</v>
+      </c>
+      <c r="K23" s="4">
+        <v>0</v>
+      </c>
+      <c r="L23" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0</v>
+      </c>
+      <c r="G24" s="4">
+        <v>0</v>
+      </c>
+      <c r="H24" s="4">
+        <v>0</v>
+      </c>
+      <c r="I24" s="4">
+        <v>0</v>
+      </c>
+      <c r="J24" s="4">
+        <v>0</v>
+      </c>
+      <c r="K24" s="4">
+        <v>0</v>
+      </c>
+      <c r="L24" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0</v>
+      </c>
+      <c r="H25" s="4">
+        <v>0</v>
+      </c>
+      <c r="I25" s="4">
+        <v>0</v>
+      </c>
+      <c r="J25" s="4">
+        <v>0</v>
+      </c>
+      <c r="K25" s="4">
+        <v>0</v>
+      </c>
+      <c r="L25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="10">
+        <v>0</v>
+      </c>
+      <c r="E26" s="10">
+        <v>0</v>
+      </c>
+      <c r="F26" s="10">
+        <v>0</v>
+      </c>
+      <c r="G26" s="10">
+        <v>0</v>
+      </c>
+      <c r="H26" s="10">
+        <v>0</v>
+      </c>
+      <c r="I26" s="10">
+        <v>0</v>
+      </c>
+      <c r="J26" s="10">
+        <v>1</v>
+      </c>
+      <c r="K26" s="10">
+        <v>0</v>
+      </c>
+      <c r="L26" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="10">
+        <v>0</v>
+      </c>
+      <c r="E27" s="10">
+        <v>0</v>
+      </c>
+      <c r="F27" s="10">
+        <v>0</v>
+      </c>
+      <c r="G27" s="10">
+        <v>0</v>
+      </c>
+      <c r="H27" s="10">
+        <v>0</v>
+      </c>
+      <c r="I27" s="10">
+        <v>0</v>
+      </c>
+      <c r="J27" s="10">
+        <v>0</v>
+      </c>
+      <c r="K27" s="10">
+        <v>1</v>
+      </c>
+      <c r="L27" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="10">
+        <v>1</v>
+      </c>
+      <c r="E28" s="10">
+        <v>0</v>
+      </c>
+      <c r="F28" s="10">
+        <v>0</v>
+      </c>
+      <c r="G28" s="10">
+        <v>0</v>
+      </c>
+      <c r="H28" s="10">
+        <v>0</v>
+      </c>
+      <c r="I28" s="10">
+        <v>0</v>
+      </c>
+      <c r="J28" s="10">
+        <v>1</v>
+      </c>
+      <c r="K28" s="10">
+        <v>0</v>
+      </c>
+      <c r="L28" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="10">
+        <v>1</v>
+      </c>
+      <c r="E29" s="10">
+        <v>0</v>
+      </c>
+      <c r="F29" s="10">
+        <v>0</v>
+      </c>
+      <c r="G29" s="10">
+        <v>0</v>
+      </c>
+      <c r="H29" s="10">
+        <v>0</v>
+      </c>
+      <c r="I29" s="10">
+        <v>0</v>
+      </c>
+      <c r="J29" s="10">
+        <v>0</v>
+      </c>
+      <c r="K29" s="10">
+        <v>1</v>
+      </c>
+      <c r="L29" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="10">
+        <v>1</v>
+      </c>
+      <c r="E30" s="10">
+        <v>0</v>
+      </c>
+      <c r="F30" s="10">
+        <v>0</v>
+      </c>
+      <c r="G30" s="10">
+        <v>0</v>
+      </c>
+      <c r="H30" s="10">
+        <v>0</v>
+      </c>
+      <c r="I30" s="10">
+        <v>0</v>
+      </c>
+      <c r="J30" s="9">
+        <v>1</v>
+      </c>
+      <c r="K30" s="10">
+        <v>1</v>
+      </c>
+      <c r="L30" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="10">
+        <v>0</v>
+      </c>
+      <c r="E31" s="10">
+        <v>0</v>
+      </c>
+      <c r="F31" s="10">
+        <v>0</v>
+      </c>
+      <c r="G31" s="10">
+        <v>0</v>
+      </c>
+      <c r="H31" s="10">
+        <v>0</v>
+      </c>
+      <c r="I31" s="10">
+        <v>0</v>
+      </c>
+      <c r="J31" s="9">
+        <v>1</v>
+      </c>
+      <c r="K31" s="10">
+        <v>1</v>
+      </c>
+      <c r="L31" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="10">
+        <v>0</v>
+      </c>
+      <c r="E32" s="10">
+        <v>0</v>
+      </c>
+      <c r="F32" s="10">
+        <v>0</v>
+      </c>
+      <c r="G32" s="10">
+        <v>0</v>
+      </c>
+      <c r="H32" s="10">
+        <v>0</v>
+      </c>
+      <c r="I32" s="10">
+        <v>0</v>
+      </c>
+      <c r="J32" s="10">
+        <v>0</v>
+      </c>
+      <c r="K32" s="10">
+        <v>0</v>
+      </c>
+      <c r="L32" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="10">
+        <v>0</v>
+      </c>
+      <c r="E33" s="10">
+        <v>0</v>
+      </c>
+      <c r="F33" s="10">
+        <v>0</v>
+      </c>
+      <c r="G33" s="10">
+        <v>0</v>
+      </c>
+      <c r="H33" s="10">
+        <v>0</v>
+      </c>
+      <c r="I33" s="10">
+        <v>1</v>
+      </c>
+      <c r="J33" s="10">
+        <v>0</v>
+      </c>
+      <c r="K33" s="10">
+        <v>0</v>
+      </c>
+      <c r="L33" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="10">
+        <v>1</v>
+      </c>
+      <c r="E34" s="10">
+        <v>0</v>
+      </c>
+      <c r="F34" s="10">
+        <v>0</v>
+      </c>
+      <c r="G34" s="10">
+        <v>0</v>
+      </c>
+      <c r="H34" s="10">
+        <v>0</v>
+      </c>
+      <c r="I34" s="10">
+        <v>0</v>
+      </c>
+      <c r="J34" s="10">
+        <v>0</v>
+      </c>
+      <c r="K34" s="10">
+        <v>0</v>
+      </c>
+      <c r="L34" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="10">
+        <v>1</v>
+      </c>
+      <c r="E35" s="10">
+        <v>1</v>
+      </c>
+      <c r="F35" s="10">
+        <v>0</v>
+      </c>
+      <c r="G35" s="10">
+        <v>0</v>
+      </c>
+      <c r="H35" s="10">
+        <v>0</v>
+      </c>
+      <c r="I35" s="10">
+        <v>0</v>
+      </c>
+      <c r="J35" s="10">
+        <v>0</v>
+      </c>
+      <c r="K35" s="10">
+        <v>0</v>
+      </c>
+      <c r="L35" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="10">
+        <v>1</v>
+      </c>
+      <c r="E36" s="10">
+        <v>1</v>
+      </c>
+      <c r="F36" s="10">
+        <v>0</v>
+      </c>
+      <c r="G36" s="10">
+        <v>0</v>
+      </c>
+      <c r="H36" s="10">
+        <v>1</v>
+      </c>
+      <c r="I36" s="10">
+        <v>0</v>
+      </c>
+      <c r="J36" s="10">
+        <v>0</v>
+      </c>
+      <c r="K36" s="10">
+        <v>0</v>
+      </c>
+      <c r="L36" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="10">
+        <v>0</v>
+      </c>
+      <c r="E37" s="10">
+        <v>0</v>
+      </c>
+      <c r="F37" s="10">
+        <v>0</v>
+      </c>
+      <c r="G37" s="10">
+        <v>0</v>
+      </c>
+      <c r="H37" s="10">
+        <v>0</v>
+      </c>
+      <c r="I37" s="10">
+        <v>0</v>
+      </c>
+      <c r="J37" s="10">
+        <v>0</v>
+      </c>
+      <c r="K37" s="10">
+        <v>0</v>
+      </c>
+      <c r="L37" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="10">
+        <v>0</v>
+      </c>
+      <c r="E38" s="10">
+        <v>1</v>
+      </c>
+      <c r="F38" s="10">
+        <v>0</v>
+      </c>
+      <c r="G38" s="10">
+        <v>0</v>
+      </c>
+      <c r="H38" s="10">
+        <v>0</v>
+      </c>
+      <c r="I38" s="10">
+        <v>0</v>
+      </c>
+      <c r="J38" s="10">
+        <v>0</v>
+      </c>
+      <c r="K38" s="10">
+        <v>0</v>
+      </c>
+      <c r="L38" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="10">
+        <v>0</v>
+      </c>
+      <c r="E39" s="10">
+        <v>1</v>
+      </c>
+      <c r="F39" s="10">
+        <v>0</v>
+      </c>
+      <c r="G39" s="10">
+        <v>0</v>
+      </c>
+      <c r="H39" s="10">
+        <v>1</v>
+      </c>
+      <c r="I39" s="10">
+        <v>0</v>
+      </c>
+      <c r="J39" s="10">
+        <v>0</v>
+      </c>
+      <c r="K39" s="10">
+        <v>0</v>
+      </c>
+      <c r="L39" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="10">
+        <v>0</v>
+      </c>
+      <c r="E40" s="10">
+        <v>1</v>
+      </c>
+      <c r="F40" s="10">
+        <v>0</v>
+      </c>
+      <c r="G40" s="10">
+        <v>0</v>
+      </c>
+      <c r="H40" s="10">
+        <v>1</v>
+      </c>
+      <c r="I40" s="10">
+        <v>0</v>
+      </c>
+      <c r="J40" s="10">
+        <v>1</v>
+      </c>
+      <c r="K40" s="10">
+        <v>0</v>
+      </c>
+      <c r="L40" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="10">
+        <v>1</v>
+      </c>
+      <c r="E41" s="10">
+        <v>0</v>
+      </c>
+      <c r="F41" s="10">
+        <v>0</v>
+      </c>
+      <c r="G41" s="10">
+        <v>0</v>
+      </c>
+      <c r="H41" s="10">
+        <v>0</v>
+      </c>
+      <c r="I41" s="10">
+        <v>0</v>
+      </c>
+      <c r="J41" s="10">
+        <v>0</v>
+      </c>
+      <c r="K41" s="10">
+        <v>0</v>
+      </c>
+      <c r="L41" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="10">
+        <v>1</v>
+      </c>
+      <c r="E42" s="10">
+        <v>1</v>
+      </c>
+      <c r="F42" s="10">
+        <v>0</v>
+      </c>
+      <c r="G42" s="10">
+        <v>0</v>
+      </c>
+      <c r="H42" s="10">
+        <v>0</v>
+      </c>
+      <c r="I42" s="10">
+        <v>0</v>
+      </c>
+      <c r="J42" s="10">
+        <v>0</v>
+      </c>
+      <c r="K42" s="10">
+        <v>0</v>
+      </c>
+      <c r="L42" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" s="10">
+        <v>1</v>
+      </c>
+      <c r="E43" s="10">
+        <v>1</v>
+      </c>
+      <c r="F43" s="10">
+        <v>0</v>
+      </c>
+      <c r="G43" s="10">
+        <v>0</v>
+      </c>
+      <c r="H43" s="10">
+        <v>1</v>
+      </c>
+      <c r="I43" s="10">
+        <v>0</v>
+      </c>
+      <c r="J43" s="10">
+        <v>0</v>
+      </c>
+      <c r="K43" s="10">
+        <v>0</v>
+      </c>
+      <c r="L43" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="10">
+        <v>0</v>
+      </c>
+      <c r="E44" s="10">
+        <v>1</v>
+      </c>
+      <c r="F44" s="10">
+        <v>0</v>
+      </c>
+      <c r="G44" s="10">
+        <v>0</v>
+      </c>
+      <c r="H44" s="10">
+        <v>1</v>
+      </c>
+      <c r="I44" s="10">
+        <v>0</v>
+      </c>
+      <c r="J44" s="10">
+        <v>1</v>
+      </c>
+      <c r="K44" s="10">
+        <v>0</v>
+      </c>
+      <c r="L44" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" s="10">
+        <v>0</v>
+      </c>
+      <c r="E45" s="10">
+        <v>0</v>
+      </c>
+      <c r="F45" s="10">
+        <v>0</v>
+      </c>
+      <c r="G45" s="10">
+        <v>0</v>
+      </c>
+      <c r="H45" s="10">
+        <v>0</v>
+      </c>
+      <c r="I45" s="10">
+        <v>0</v>
+      </c>
+      <c r="J45" s="10">
+        <v>0</v>
+      </c>
+      <c r="K45" s="10">
+        <v>0</v>
+      </c>
+      <c r="L45" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" s="10">
+        <v>0</v>
+      </c>
+      <c r="E46" s="10">
+        <v>1</v>
+      </c>
+      <c r="F46" s="10">
+        <v>0</v>
+      </c>
+      <c r="G46" s="10">
+        <v>0</v>
+      </c>
+      <c r="H46" s="10">
+        <v>1</v>
+      </c>
+      <c r="I46" s="10">
+        <v>0</v>
+      </c>
+      <c r="J46" s="10">
+        <v>0</v>
+      </c>
+      <c r="K46" s="10">
+        <v>0</v>
+      </c>
+      <c r="L46" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" s="10">
+        <v>0</v>
+      </c>
+      <c r="E47" s="10">
+        <v>1</v>
+      </c>
+      <c r="F47" s="10">
+        <v>0</v>
+      </c>
+      <c r="G47" s="10">
+        <v>0</v>
+      </c>
+      <c r="H47" s="10">
+        <v>0</v>
+      </c>
+      <c r="I47" s="10">
+        <v>0</v>
+      </c>
+      <c r="J47" s="10">
+        <v>0</v>
+      </c>
+      <c r="K47" s="10">
+        <v>0</v>
+      </c>
+      <c r="L47" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" s="10">
+        <v>1</v>
+      </c>
+      <c r="E48" s="10">
+        <v>0</v>
+      </c>
+      <c r="F48" s="10">
+        <v>0</v>
+      </c>
+      <c r="G48" s="10">
+        <v>0</v>
+      </c>
+      <c r="H48" s="10">
+        <v>0</v>
+      </c>
+      <c r="I48" s="10">
+        <v>0</v>
+      </c>
+      <c r="J48" s="10">
+        <v>0</v>
+      </c>
+      <c r="K48" s="10">
+        <v>0</v>
+      </c>
+      <c r="L48" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="4">
+        <v>0</v>
+      </c>
+      <c r="E49" s="4">
+        <v>0</v>
+      </c>
+      <c r="F49" s="4">
+        <v>0</v>
+      </c>
+      <c r="G49" s="4">
+        <v>0</v>
+      </c>
+      <c r="H49" s="4">
+        <v>0</v>
+      </c>
+      <c r="I49" s="4">
+        <v>0</v>
+      </c>
+      <c r="J49" s="4">
+        <v>0</v>
+      </c>
+      <c r="K49" s="4">
+        <v>0</v>
+      </c>
+      <c r="L49" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="4">
+        <v>0</v>
+      </c>
+      <c r="E50" s="4">
+        <v>1</v>
+      </c>
+      <c r="F50" s="4">
+        <v>0</v>
+      </c>
+      <c r="G50" s="4">
+        <v>0</v>
+      </c>
+      <c r="H50" s="4">
+        <v>0</v>
+      </c>
+      <c r="I50" s="4">
+        <v>0</v>
+      </c>
+      <c r="J50" s="4">
+        <v>0</v>
+      </c>
+      <c r="K50" s="4">
+        <v>0</v>
+      </c>
+      <c r="L50" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="4">
+        <v>0</v>
+      </c>
+      <c r="E51" s="4">
+        <v>1</v>
+      </c>
+      <c r="F51" s="4">
+        <v>1</v>
+      </c>
+      <c r="G51" s="4">
+        <v>0</v>
+      </c>
+      <c r="H51" s="4">
+        <v>0</v>
+      </c>
+      <c r="I51" s="4">
+        <v>0</v>
+      </c>
+      <c r="J51" s="4">
+        <v>0</v>
+      </c>
+      <c r="K51" s="4">
+        <v>0</v>
+      </c>
+      <c r="L51" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" s="4">
+        <v>0</v>
+      </c>
+      <c r="E52" s="4">
+        <v>1</v>
+      </c>
+      <c r="F52" s="4">
+        <v>0</v>
+      </c>
+      <c r="G52" s="4">
+        <v>1</v>
+      </c>
+      <c r="H52" s="4">
+        <v>0</v>
+      </c>
+      <c r="I52" s="4">
+        <v>0</v>
+      </c>
+      <c r="J52" s="4">
+        <v>0</v>
+      </c>
+      <c r="K52" s="4">
+        <v>0</v>
+      </c>
+      <c r="L52" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>16</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="4">
+        <v>0</v>
+      </c>
+      <c r="E53" s="4">
+        <v>1</v>
+      </c>
+      <c r="F53" s="4">
+        <v>1</v>
+      </c>
+      <c r="G53" s="4">
+        <v>0</v>
+      </c>
+      <c r="H53" s="4">
+        <v>0</v>
+      </c>
+      <c r="I53" s="4">
+        <v>0</v>
+      </c>
+      <c r="J53" s="4">
+        <v>1</v>
+      </c>
+      <c r="K53" s="4">
+        <v>0</v>
+      </c>
+      <c r="L53" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>22</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" t="s">
+        <v>16</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>22</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="9">
+        <v>1</v>
+      </c>
+      <c r="E57" s="9">
+        <v>0</v>
+      </c>
+      <c r="F57" s="9">
+        <v>0</v>
+      </c>
+      <c r="G57" s="9">
+        <v>0</v>
+      </c>
+      <c r="H57" s="9">
+        <v>0</v>
+      </c>
+      <c r="I57" s="9">
+        <v>0</v>
+      </c>
+      <c r="J57" s="9">
+        <v>0</v>
+      </c>
+      <c r="K57" s="9">
+        <v>0</v>
+      </c>
+      <c r="L57" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="9">
+        <v>0</v>
+      </c>
+      <c r="E58" s="9">
+        <v>0</v>
+      </c>
+      <c r="F58" s="9">
+        <v>0</v>
+      </c>
+      <c r="G58" s="9">
+        <v>0</v>
+      </c>
+      <c r="H58" s="9">
+        <v>0</v>
+      </c>
+      <c r="I58" s="10">
+        <v>1</v>
+      </c>
+      <c r="J58" s="10">
+        <v>0</v>
+      </c>
+      <c r="K58" s="10">
+        <v>0</v>
+      </c>
+      <c r="L58" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="9">
+        <v>1</v>
+      </c>
+      <c r="E59" s="9">
+        <v>0</v>
+      </c>
+      <c r="F59" s="9">
+        <v>0</v>
+      </c>
+      <c r="G59" s="9">
+        <v>0</v>
+      </c>
+      <c r="H59" s="9">
+        <v>0</v>
+      </c>
+      <c r="I59" s="10">
+        <v>0</v>
+      </c>
+      <c r="J59" s="10">
+        <v>1</v>
+      </c>
+      <c r="K59" s="10">
+        <v>0</v>
+      </c>
+      <c r="L59" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="9">
+        <v>1</v>
+      </c>
+      <c r="E60" s="9">
+        <v>0</v>
+      </c>
+      <c r="F60" s="9">
+        <v>0</v>
+      </c>
+      <c r="G60" s="9">
+        <v>0</v>
+      </c>
+      <c r="H60" s="9">
+        <v>0</v>
+      </c>
+      <c r="I60" s="9">
+        <v>0</v>
+      </c>
+      <c r="J60" s="9">
+        <v>0</v>
+      </c>
+      <c r="K60" s="9">
+        <v>1</v>
+      </c>
+      <c r="L60" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" s="9">
+        <v>1</v>
+      </c>
+      <c r="E61" s="9">
+        <v>0</v>
+      </c>
+      <c r="F61" s="9">
+        <v>0</v>
+      </c>
+      <c r="G61" s="9">
+        <v>0</v>
+      </c>
+      <c r="H61" s="9">
+        <v>0</v>
+      </c>
+      <c r="I61" s="9">
+        <v>0</v>
+      </c>
+      <c r="J61" s="9">
+        <v>1</v>
+      </c>
+      <c r="K61" s="9">
+        <v>1</v>
+      </c>
+      <c r="L61" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" s="9">
+        <v>0</v>
+      </c>
+      <c r="E62" s="9">
+        <v>0</v>
+      </c>
+      <c r="F62" s="9">
+        <v>0</v>
+      </c>
+      <c r="G62" s="9">
+        <v>0</v>
+      </c>
+      <c r="H62" s="9">
+        <v>0</v>
+      </c>
+      <c r="I62" s="9">
+        <v>0</v>
+      </c>
+      <c r="J62" s="9">
+        <v>1</v>
+      </c>
+      <c r="K62" s="9">
+        <v>0</v>
+      </c>
+      <c r="L62" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="9">
+        <v>0</v>
+      </c>
+      <c r="E63" s="9">
+        <v>0</v>
+      </c>
+      <c r="F63" s="9">
+        <v>0</v>
+      </c>
+      <c r="G63" s="9">
+        <v>0</v>
+      </c>
+      <c r="H63" s="9">
+        <v>0</v>
+      </c>
+      <c r="I63" s="9">
+        <v>0</v>
+      </c>
+      <c r="J63" s="9">
+        <v>0</v>
+      </c>
+      <c r="K63" s="9">
+        <v>1</v>
+      </c>
+      <c r="L63" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64" s="9">
+        <v>0</v>
+      </c>
+      <c r="E64" s="9">
+        <v>0</v>
+      </c>
+      <c r="F64" s="9">
+        <v>0</v>
+      </c>
+      <c r="G64" s="9">
+        <v>0</v>
+      </c>
+      <c r="H64" s="9">
+        <v>0</v>
+      </c>
+      <c r="I64" s="9">
+        <v>0</v>
+      </c>
+      <c r="J64" s="9">
+        <v>1</v>
+      </c>
+      <c r="K64" s="9">
+        <v>1</v>
+      </c>
+      <c r="L64" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65" s="9">
+        <v>0</v>
+      </c>
+      <c r="E65" s="9">
+        <v>0</v>
+      </c>
+      <c r="F65" s="9">
+        <v>0</v>
+      </c>
+      <c r="G65" s="9">
+        <v>0</v>
+      </c>
+      <c r="H65" s="9">
+        <v>0</v>
+      </c>
+      <c r="I65" s="9">
+        <v>0</v>
+      </c>
+      <c r="J65" s="9">
+        <v>0</v>
+      </c>
+      <c r="K65" s="9">
+        <v>0</v>
+      </c>
+      <c r="L65" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>23</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C66" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>23</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C67" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67" s="3">
+        <v>1</v>
+      </c>
+      <c r="J67" s="3">
+        <v>0</v>
+      </c>
+      <c r="K67" s="3">
+        <v>0</v>
+      </c>
+      <c r="L67" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>23</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C68" t="s">
+        <v>14</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68" s="3">
+        <v>0</v>
+      </c>
+      <c r="J68" s="3">
+        <v>1</v>
+      </c>
+      <c r="K68" s="3">
+        <v>0</v>
+      </c>
+      <c r="L68" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>23</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C69" t="s">
+        <v>14</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+      <c r="K69">
+        <v>1</v>
+      </c>
+      <c r="L69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>23</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C70" t="s">
+        <v>14</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>1</v>
+      </c>
+      <c r="K70">
+        <v>1</v>
+      </c>
+      <c r="L70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>23</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C71" t="s">
+        <v>14</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>1</v>
+      </c>
+      <c r="K71">
+        <v>0</v>
+      </c>
+      <c r="L71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>23</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C72" t="s">
+        <v>14</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+      <c r="K72">
+        <v>1</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>23</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C73" t="s">
+        <v>14</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>1</v>
+      </c>
+      <c r="K73">
+        <v>1</v>
+      </c>
+      <c r="L73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>23</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C74" t="s">
+        <v>14</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+      <c r="J74">
+        <v>0</v>
+      </c>
+      <c r="K74">
+        <v>0</v>
+      </c>
+      <c r="L74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D75" s="9">
+        <v>1</v>
+      </c>
+      <c r="E75" s="9">
+        <v>1</v>
+      </c>
+      <c r="F75" s="9">
+        <v>0</v>
+      </c>
+      <c r="G75" s="9">
+        <v>0</v>
+      </c>
+      <c r="H75" s="9">
+        <v>1</v>
+      </c>
+      <c r="I75" s="9">
+        <v>0</v>
+      </c>
+      <c r="J75" s="9">
+        <v>0</v>
+      </c>
+      <c r="K75" s="9">
+        <v>0</v>
+      </c>
+      <c r="L75" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" s="9" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D76" s="9">
+        <v>0</v>
+      </c>
+      <c r="E76" s="9">
+        <v>1</v>
+      </c>
+      <c r="F76" s="9">
+        <v>0</v>
+      </c>
+      <c r="G76" s="9">
+        <v>0</v>
+      </c>
+      <c r="H76" s="9">
+        <v>1</v>
+      </c>
+      <c r="I76" s="9">
+        <v>0</v>
+      </c>
+      <c r="J76" s="9">
+        <v>1</v>
+      </c>
+      <c r="K76" s="9">
+        <v>0</v>
+      </c>
+      <c r="L76" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D77" s="9">
+        <v>1</v>
+      </c>
+      <c r="E77" s="9">
+        <v>1</v>
+      </c>
+      <c r="F77" s="9">
+        <v>0</v>
+      </c>
+      <c r="G77" s="9">
+        <v>0</v>
+      </c>
+      <c r="H77" s="9">
+        <v>0</v>
+      </c>
+      <c r="I77" s="9">
+        <v>0</v>
+      </c>
+      <c r="J77" s="9">
+        <v>0</v>
+      </c>
+      <c r="K77" s="9">
+        <v>0</v>
+      </c>
+      <c r="L77" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B78" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D78" s="9">
+        <v>0</v>
+      </c>
+      <c r="E78" s="9">
+        <v>1</v>
+      </c>
+      <c r="F78" s="9">
+        <v>0</v>
+      </c>
+      <c r="G78" s="9">
+        <v>0</v>
+      </c>
+      <c r="H78" s="9">
+        <v>1</v>
+      </c>
+      <c r="I78" s="9">
+        <v>0</v>
+      </c>
+      <c r="J78" s="9">
+        <v>0</v>
+      </c>
+      <c r="K78" s="9">
+        <v>0</v>
+      </c>
+      <c r="L78" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D79" s="9">
+        <v>0</v>
+      </c>
+      <c r="E79" s="9">
+        <v>1</v>
+      </c>
+      <c r="F79" s="9">
+        <v>0</v>
+      </c>
+      <c r="G79" s="9">
+        <v>0</v>
+      </c>
+      <c r="H79" s="9">
+        <v>0</v>
+      </c>
+      <c r="I79" s="9">
+        <v>0</v>
+      </c>
+      <c r="J79" s="9">
+        <v>0</v>
+      </c>
+      <c r="K79" s="9">
+        <v>0</v>
+      </c>
+      <c r="L79" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D80" s="9">
+        <v>1</v>
+      </c>
+      <c r="E80" s="9">
+        <v>0</v>
+      </c>
+      <c r="F80" s="9">
+        <v>0</v>
+      </c>
+      <c r="G80" s="9">
+        <v>0</v>
+      </c>
+      <c r="H80" s="9">
+        <v>0</v>
+      </c>
+      <c r="I80" s="9">
+        <v>0</v>
+      </c>
+      <c r="J80" s="9">
+        <v>0</v>
+      </c>
+      <c r="K80" s="9">
+        <v>0</v>
+      </c>
+      <c r="L80" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D81" s="9">
+        <v>0</v>
+      </c>
+      <c r="E81" s="9">
+        <v>0</v>
+      </c>
+      <c r="F81" s="9">
+        <v>0</v>
+      </c>
+      <c r="G81" s="9">
+        <v>0</v>
+      </c>
+      <c r="H81" s="9">
+        <v>0</v>
+      </c>
+      <c r="I81" s="9">
+        <v>0</v>
+      </c>
+      <c r="J81" s="10">
+        <v>0</v>
+      </c>
+      <c r="K81" s="9">
+        <v>0</v>
+      </c>
+      <c r="L81" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B82" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D82" s="9">
+        <v>1</v>
+      </c>
+      <c r="E82" s="9">
+        <v>1</v>
+      </c>
+      <c r="F82" s="9">
+        <v>0</v>
+      </c>
+      <c r="G82" s="9">
+        <v>0</v>
+      </c>
+      <c r="H82" s="9">
+        <v>1</v>
+      </c>
+      <c r="I82" s="9">
+        <v>0</v>
+      </c>
+      <c r="J82" s="9">
+        <v>0</v>
+      </c>
+      <c r="K82" s="9">
+        <v>0</v>
+      </c>
+      <c r="L82" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B83" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D83" s="9">
+        <v>0</v>
+      </c>
+      <c r="E83" s="9">
+        <v>1</v>
+      </c>
+      <c r="F83" s="9">
+        <v>0</v>
+      </c>
+      <c r="G83" s="9">
+        <v>0</v>
+      </c>
+      <c r="H83" s="9">
+        <v>1</v>
+      </c>
+      <c r="I83" s="9">
+        <v>0</v>
+      </c>
+      <c r="J83" s="9">
+        <v>1</v>
+      </c>
+      <c r="K83" s="9">
+        <v>0</v>
+      </c>
+      <c r="L83" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B84" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D84" s="9">
+        <v>1</v>
+      </c>
+      <c r="E84" s="9">
+        <v>1</v>
+      </c>
+      <c r="F84" s="9">
+        <v>0</v>
+      </c>
+      <c r="G84" s="9">
+        <v>0</v>
+      </c>
+      <c r="H84" s="9">
+        <v>0</v>
+      </c>
+      <c r="I84" s="9">
+        <v>0</v>
+      </c>
+      <c r="J84" s="9">
+        <v>0</v>
+      </c>
+      <c r="K84" s="9">
+        <v>0</v>
+      </c>
+      <c r="L84" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C85" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D85" s="9">
+        <v>0</v>
+      </c>
+      <c r="E85" s="9">
+        <v>1</v>
+      </c>
+      <c r="F85" s="9">
+        <v>0</v>
+      </c>
+      <c r="G85" s="9">
+        <v>0</v>
+      </c>
+      <c r="H85" s="9">
+        <v>1</v>
+      </c>
+      <c r="I85" s="9">
+        <v>0</v>
+      </c>
+      <c r="J85" s="9">
+        <v>0</v>
+      </c>
+      <c r="K85" s="9">
+        <v>0</v>
+      </c>
+      <c r="L85" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B86" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D86" s="9">
+        <v>0</v>
+      </c>
+      <c r="E86" s="9">
+        <v>1</v>
+      </c>
+      <c r="F86" s="9">
+        <v>0</v>
+      </c>
+      <c r="G86" s="9">
+        <v>0</v>
+      </c>
+      <c r="H86" s="9">
+        <v>0</v>
+      </c>
+      <c r="I86" s="9">
+        <v>0</v>
+      </c>
+      <c r="J86" s="9">
+        <v>0</v>
+      </c>
+      <c r="K86" s="9">
+        <v>0</v>
+      </c>
+      <c r="L86" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B87" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D87" s="9">
+        <v>1</v>
+      </c>
+      <c r="E87" s="9">
+        <v>0</v>
+      </c>
+      <c r="F87" s="9">
+        <v>0</v>
+      </c>
+      <c r="G87" s="9">
+        <v>0</v>
+      </c>
+      <c r="H87" s="9">
+        <v>0</v>
+      </c>
+      <c r="I87" s="9">
+        <v>0</v>
+      </c>
+      <c r="J87" s="9">
+        <v>0</v>
+      </c>
+      <c r="K87" s="9">
+        <v>0</v>
+      </c>
+      <c r="L87" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B88" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D88" s="9">
+        <v>0</v>
+      </c>
+      <c r="E88" s="9">
+        <v>0</v>
+      </c>
+      <c r="F88" s="9">
+        <v>0</v>
+      </c>
+      <c r="G88" s="9">
+        <v>0</v>
+      </c>
+      <c r="H88" s="9">
+        <v>0</v>
+      </c>
+      <c r="I88" s="9">
+        <v>0</v>
+      </c>
+      <c r="J88" s="10">
+        <v>0</v>
+      </c>
+      <c r="K88" s="9">
+        <v>0</v>
+      </c>
+      <c r="L88" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B89" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C89" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D89" s="10">
+        <v>0</v>
+      </c>
+      <c r="E89" s="10">
+        <v>1</v>
+      </c>
+      <c r="F89" s="10">
+        <v>1</v>
+      </c>
+      <c r="G89" s="10">
+        <v>0</v>
+      </c>
+      <c r="H89" s="10">
+        <v>0</v>
+      </c>
+      <c r="I89" s="10">
+        <v>0</v>
+      </c>
+      <c r="J89" s="10">
+        <v>0</v>
+      </c>
+      <c r="K89" s="10">
+        <v>0</v>
+      </c>
+      <c r="L89" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B90" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C90" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D90" s="10">
+        <v>0</v>
+      </c>
+      <c r="E90" s="10">
+        <v>1</v>
+      </c>
+      <c r="F90" s="10">
+        <v>0</v>
+      </c>
+      <c r="G90" s="10">
+        <v>1</v>
+      </c>
+      <c r="H90" s="10">
+        <v>0</v>
+      </c>
+      <c r="I90" s="10">
+        <v>0</v>
+      </c>
+      <c r="J90" s="10">
+        <v>0</v>
+      </c>
+      <c r="K90" s="10">
+        <v>0</v>
+      </c>
+      <c r="L90" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B91" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C91" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D91" s="10">
+        <v>0</v>
+      </c>
+      <c r="E91" s="10">
+        <v>1</v>
+      </c>
+      <c r="F91" s="10">
+        <v>1</v>
+      </c>
+      <c r="G91" s="10">
+        <v>0</v>
+      </c>
+      <c r="H91" s="10">
+        <v>0</v>
+      </c>
+      <c r="I91" s="10">
+        <v>0</v>
+      </c>
+      <c r="J91" s="10">
+        <v>1</v>
+      </c>
+      <c r="K91" s="10">
+        <v>0</v>
+      </c>
+      <c r="L91" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B92" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C92" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D92" s="10">
+        <v>0</v>
+      </c>
+      <c r="E92" s="10">
+        <v>0</v>
+      </c>
+      <c r="F92" s="10">
+        <v>0</v>
+      </c>
+      <c r="G92" s="10">
+        <v>0</v>
+      </c>
+      <c r="H92" s="10">
+        <v>0</v>
+      </c>
+      <c r="I92" s="10">
+        <v>0</v>
+      </c>
+      <c r="J92" s="10">
+        <v>0</v>
+      </c>
+      <c r="K92" s="10">
+        <v>0</v>
+      </c>
+      <c r="L92" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B93" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C93" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D93" s="10">
+        <v>0</v>
+      </c>
+      <c r="E93" s="10">
+        <v>1</v>
+      </c>
+      <c r="F93" s="10">
+        <v>0</v>
+      </c>
+      <c r="G93" s="10">
+        <v>0</v>
+      </c>
+      <c r="H93" s="10">
+        <v>0</v>
+      </c>
+      <c r="I93" s="10">
+        <v>0</v>
+      </c>
+      <c r="J93" s="10">
+        <v>0</v>
+      </c>
+      <c r="K93" s="10">
+        <v>0</v>
+      </c>
+      <c r="L93" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B94" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C94" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D94" s="10">
+        <v>1</v>
+      </c>
+      <c r="E94" s="10">
+        <v>0</v>
+      </c>
+      <c r="F94" s="10">
+        <v>0</v>
+      </c>
+      <c r="G94" s="10">
+        <v>0</v>
+      </c>
+      <c r="H94" s="10">
+        <v>0</v>
+      </c>
+      <c r="I94" s="10">
+        <v>0</v>
+      </c>
+      <c r="J94" s="10">
+        <v>0</v>
+      </c>
+      <c r="K94" s="10">
+        <v>0</v>
+      </c>
+      <c r="L94" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>23</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C95" t="s">
+        <v>15</v>
+      </c>
+      <c r="D95" s="10">
+        <v>0</v>
+      </c>
+      <c r="E95" s="10">
+        <v>1</v>
+      </c>
+      <c r="F95" s="10">
+        <v>1</v>
+      </c>
+      <c r="G95" s="10">
+        <v>0</v>
+      </c>
+      <c r="H95" s="10">
+        <v>0</v>
+      </c>
+      <c r="I95" s="10">
+        <v>0</v>
+      </c>
+      <c r="J95" s="10">
+        <v>0</v>
+      </c>
+      <c r="K95" s="10">
+        <v>0</v>
+      </c>
+      <c r="L95" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>23</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C96" t="s">
+        <v>15</v>
+      </c>
+      <c r="D96" s="10">
+        <v>0</v>
+      </c>
+      <c r="E96" s="10">
+        <v>1</v>
+      </c>
+      <c r="F96" s="10">
+        <v>0</v>
+      </c>
+      <c r="G96" s="10">
+        <v>1</v>
+      </c>
+      <c r="H96" s="10">
+        <v>0</v>
+      </c>
+      <c r="I96" s="10">
+        <v>0</v>
+      </c>
+      <c r="J96" s="10">
+        <v>0</v>
+      </c>
+      <c r="K96" s="10">
+        <v>0</v>
+      </c>
+      <c r="L96" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>23</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C97" t="s">
+        <v>15</v>
+      </c>
+      <c r="D97" s="10">
+        <v>0</v>
+      </c>
+      <c r="E97" s="10">
+        <v>1</v>
+      </c>
+      <c r="F97" s="10">
+        <v>1</v>
+      </c>
+      <c r="G97" s="10">
+        <v>0</v>
+      </c>
+      <c r="H97" s="10">
+        <v>0</v>
+      </c>
+      <c r="I97" s="10">
+        <v>0</v>
+      </c>
+      <c r="J97" s="10">
+        <v>1</v>
+      </c>
+      <c r="K97" s="10">
+        <v>0</v>
+      </c>
+      <c r="L97" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>23</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C98" t="s">
+        <v>15</v>
+      </c>
+      <c r="D98" s="10">
+        <v>0</v>
+      </c>
+      <c r="E98" s="10">
+        <v>0</v>
+      </c>
+      <c r="F98" s="10">
+        <v>0</v>
+      </c>
+      <c r="G98" s="10">
+        <v>0</v>
+      </c>
+      <c r="H98" s="10">
+        <v>0</v>
+      </c>
+      <c r="I98" s="10">
+        <v>0</v>
+      </c>
+      <c r="J98" s="10">
+        <v>0</v>
+      </c>
+      <c r="K98" s="10">
+        <v>0</v>
+      </c>
+      <c r="L98" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>23</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C99" t="s">
+        <v>15</v>
+      </c>
+      <c r="D99" s="10">
+        <v>0</v>
+      </c>
+      <c r="E99" s="10">
+        <v>1</v>
+      </c>
+      <c r="F99" s="10">
+        <v>0</v>
+      </c>
+      <c r="G99" s="10">
+        <v>0</v>
+      </c>
+      <c r="H99" s="10">
+        <v>0</v>
+      </c>
+      <c r="I99" s="10">
+        <v>0</v>
+      </c>
+      <c r="J99" s="10">
+        <v>0</v>
+      </c>
+      <c r="K99" s="10">
+        <v>0</v>
+      </c>
+      <c r="L99" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>23</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C100" t="s">
+        <v>15</v>
+      </c>
+      <c r="D100" s="10">
+        <v>1</v>
+      </c>
+      <c r="E100" s="10">
+        <v>0</v>
+      </c>
+      <c r="F100" s="10">
+        <v>0</v>
+      </c>
+      <c r="G100" s="10">
+        <v>0</v>
+      </c>
+      <c r="H100" s="10">
+        <v>0</v>
+      </c>
+      <c r="I100" s="10">
+        <v>0</v>
+      </c>
+      <c r="J100" s="10">
+        <v>0</v>
+      </c>
+      <c r="K100" s="10">
+        <v>0</v>
+      </c>
+      <c r="L100" s="10">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>